<commit_message>
Atualização: gráfico completo Petrobras e código da aula
</commit_message>
<xml_diff>
--- a/datasets/petrobras.xlsx
+++ b/datasets/petrobras.xlsx
@@ -1,36 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\trabalho\Livro Pyhton_Merc_Fin\Cap1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cassio49734596\Desktop\AULA_2_BRACH\datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24F9599B-ADE5-4EE6-A625-1C7AF7ABF556}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{21B01B20-B0F4-416B-8781-1EF19A701CB0}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7995"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -96,7 +90,7 @@
         <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent1>
       <a:accent2>
         <a:srgbClr val="ED7D31"/>
@@ -108,7 +102,7 @@
         <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent5>
       <a:accent6>
         <a:srgbClr val="70AD47"/>
@@ -155,23 +149,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -207,23 +184,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -375,111 +335,111 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCFC2604-4E5F-4035-B252-E79B16B86D33}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M21" sqref="M21"/>
+      <selection sqref="A1:A20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>1.31</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1.34</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1.42</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1.4</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1.42</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>1.4</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>1.47</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>1.45</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>1.48</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>1.42</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>1.34</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>1.34</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>1.35</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>1.35</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>1.36</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>1.32</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>1.24</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>1.22</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>1.27</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>1.26</v>
       </c>

</xml_diff>